<commit_message>
download excel file with data #9
</commit_message>
<xml_diff>
--- a/uploads/allOprihods.xlsx
+++ b/uploads/allOprihods.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -717,9 +717,44 @@
         <v/>
       </c>
     </row>
+    <row r="10">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10" t="str">
+        <v>08.09.2023, 15:32:47</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Борт 50.21.3,5</v>
+      </c>
+      <c r="E10" t="str">
+        <v>черный</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Продукция Плиточка/Бордюры</v>
+      </c>
+      <c r="I10" t="str">
+        <v>08.09.2023</v>
+      </c>
+      <c r="J10" t="str">
+        <v>15:32:41</v>
+      </c>
+      <c r="K10" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
download file excel from bot space
</commit_message>
<xml_diff>
--- a/uploads/allOprihods.xlsx
+++ b/uploads/allOprihods.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -752,9 +752,79 @@
         <v/>
       </c>
     </row>
+    <row r="11">
+      <c r="A11">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>61</v>
+      </c>
+      <c r="C11" t="str">
+        <v>09.09.2023, 22:59:56</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Блок Польский</v>
+      </c>
+      <c r="E11" t="str">
+        <v>туман</v>
+      </c>
+      <c r="F11" t="str">
+        <v>УЦЕНКА</v>
+      </c>
+      <c r="G11">
+        <v>680</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Продукция Плиточка/Блоки заборные</v>
+      </c>
+      <c r="I11" t="str">
+        <v>08.09.2023</v>
+      </c>
+      <c r="J11" t="str">
+        <v>17:38:06</v>
+      </c>
+      <c r="K11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>162</v>
+      </c>
+      <c r="C12" t="str">
+        <v>09.09.2023, 22:59:56</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Старый город</v>
+      </c>
+      <c r="E12" t="str">
+        <v>оливковый</v>
+      </c>
+      <c r="F12" t="str">
+        <v>УЦЕНКА</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="str">
+        <v>Продукция Плиточка/Тротуарная плитка/Вибропресс/Старый город</v>
+      </c>
+      <c r="I12" t="str">
+        <v>09.09.2023</v>
+      </c>
+      <c r="J12" t="str">
+        <v>22:59:42</v>
+      </c>
+      <c r="K12" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>